<commit_message>
Testdaten geändert PRäsi eingefügt
</commit_message>
<xml_diff>
--- a/documents/test/1_Testing_Gast_KA.xlsx
+++ b/documents/test/1_Testing_Gast_KA.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
   <si>
     <t>Gast</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Anmelden</t>
   </si>
   <si>
-    <t>User erfolgreich eingeloggt</t>
-  </si>
-  <si>
     <t>Nutzer</t>
   </si>
   <si>
@@ -128,6 +125,12 @@
   </si>
   <si>
     <t>Getestet von KA</t>
+  </si>
+  <si>
+    <t>Anmelde-Seite angezeigt</t>
+  </si>
+  <si>
+    <t>Anmelde-Seite wird angezeigt</t>
   </si>
 </sst>
 </file>
@@ -654,7 +657,7 @@
   <dimension ref="B1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,13 +677,13 @@
     <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="E2" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -752,10 +755,10 @@
         <v>14</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
@@ -767,19 +770,19 @@
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
@@ -791,19 +794,19 @@
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
@@ -815,19 +818,19 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
@@ -839,25 +842,25 @@
     </row>
     <row r="11" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="G11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I11" s="11">
         <v>42605</v>
@@ -865,19 +868,19 @@
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
@@ -889,19 +892,19 @@
     </row>
     <row r="13" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">

</xml_diff>